<commit_message>
with multivarite multilevel analysis
</commit_message>
<xml_diff>
--- a/Data/statistics_results.xlsx
+++ b/Data/statistics_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\DataMohammed\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3727FB-F517-4FEC-84F2-763F604BB0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3035FBC6-E16D-4797-9E33-E821C30A56D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,161 +174,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>13935</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA3257E5-EA4D-FC1C-5947-8AD62AC848CF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="30480" y="2377441"/>
-          <a:ext cx="5257800" cy="3244814"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>45721</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>154665</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5B4AA8-52D9-CC70-A23F-A025F369AF72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5425440" y="2324101"/>
-          <a:ext cx="5288280" cy="3263624"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>143127</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{365EDFA5-47F9-13BE-42A4-4C799EFA2654}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10904220" y="2453641"/>
-          <a:ext cx="5059680" cy="3122546"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
@@ -1055,6 +900,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>